<commit_message>
changed sheet2's name from chinese to english.
</commit_message>
<xml_diff>
--- a/ISIC_to_ROCSIC.xlsx
+++ b/ISIC_to_ROCSIC.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User_Data\Desktop\研究資料\HWT\工商普查資料處理\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52EF879-7B9F-4108-A55E-6D4B87A78AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0274765-F590-49E1-A72E-04B409E7FBFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
-    <sheet name="工作表2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>